<commit_message>
WBS och aktivitetslista samt som csv-fil
</commit_message>
<xml_diff>
--- a/Bolaget/Planering/A1 WBS & Aktivitetslista/Aktivitetslista.xlsx
+++ b/Bolaget/Planering/A1 WBS & Aktivitetslista/Aktivitetslista.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t xml:space="preserve">Färdigställ rapport och skicka in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt:</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -391,21 +394,91 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -434,7 +507,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,6 +518,90 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -456,6 +613,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -466,47 +683,47 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.69387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="89.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="20.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.63775510204082"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="89.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.64"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -515,9 +732,13 @@
       <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -526,9 +747,13 @@
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -537,21 +762,21 @@
       <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -560,21 +785,21 @@
       <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -583,21 +808,21 @@
       <c r="C6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -606,21 +831,21 @@
       <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -629,21 +854,21 @@
       <c r="C8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="14" t="n">
         <v>24</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -652,21 +877,21 @@
       <c r="C9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -675,9 +900,13 @@
       <c r="C10" s="0" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -686,21 +915,21 @@
       <c r="C11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -709,9 +938,13 @@
       <c r="C12" s="0" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -720,21 +953,21 @@
       <c r="C13" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -743,21 +976,21 @@
       <c r="C14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -766,21 +999,21 @@
       <c r="C15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -789,21 +1022,21 @@
       <c r="C16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -812,21 +1045,21 @@
       <c r="C17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
@@ -835,9 +1068,13 @@
       <c r="C18" s="0" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="0" t="s">
@@ -846,21 +1083,21 @@
       <c r="C19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="0" t="s">
@@ -869,21 +1106,21 @@
       <c r="C20" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="14" t="n">
         <v>15</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -892,44 +1129,44 @@
       <c r="C21" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E22" s="0" t="n">
+      <c r="D22" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="n">
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -938,9 +1175,13 @@
       <c r="C23" s="0" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="0" t="s">
@@ -949,9 +1190,13 @@
       <c r="C24" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="0" t="s">
@@ -960,21 +1205,21 @@
       <c r="C25" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G25" s="2" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="G25" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B26" s="0" t="s">
@@ -983,21 +1228,21 @@
       <c r="C26" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -1006,21 +1251,21 @@
       <c r="C27" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="14" t="n">
         <v>1.5</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="0" t="s">
@@ -1029,21 +1274,21 @@
       <c r="C28" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F28" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F28" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
         <v>89</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -1052,21 +1297,21 @@
       <c r="C29" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="14" t="n">
         <v>1.5</v>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="G29" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -1075,21 +1320,21 @@
       <c r="C30" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="0" t="s">
@@ -1098,21 +1343,21 @@
       <c r="C31" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="13" t="n">
         <v>2</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B32" s="0" t="s">
@@ -1121,41 +1366,42 @@
       <c r="C32" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="13" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="14" t="n">
         <v>0.5</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="17" t="n">
         <v>0.5</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="19" t="n">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="n">
         <v>3</v>
       </c>
       <c r="B34" s="0" t="s">
@@ -1164,12 +1410,14 @@
       <c r="C34" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="D34" s="13"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="0" t="s">
@@ -1178,48 +1426,51 @@
       <c r="C35" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="13" t="n">
         <v>3</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F35" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G35" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="D36" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E36" s="0" t="n">
+      <c r="D36" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="F36" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G36" s="2" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="0" t="n">
+      <c r="F36" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D37" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="22" t="n">
         <f aca="false">SUM(E4:E36)</f>
         <v>80</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="23" t="n">
         <f aca="false">SUM(F4:F36)</f>
         <v>196</v>
       </c>

</xml_diff>